<commit_message>
update app.py missions.xlsx setings.py
</commit_message>
<xml_diff>
--- a/missions.xlsx
+++ b/missions.xlsx
@@ -17,8 +17,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -78,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -87,7 +87,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,10 +561,10 @@
           <t>14:16:14</t>
         </is>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>45505</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <v>45506</v>
       </c>
       <c r="F2" t="inlineStr">
@@ -621,10 +622,10 @@
           <t>14:17:19</t>
         </is>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>45505</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="5" t="n">
         <v>45505</v>
       </c>
       <c r="F3" t="inlineStr">
@@ -682,10 +683,10 @@
           <t>14:20:53</t>
         </is>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>45505</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="5" t="n">
         <v>45505</v>
       </c>
       <c r="F4" t="inlineStr">
@@ -743,10 +744,10 @@
           <t>20:57:09</t>
         </is>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>45506</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>45506</v>
       </c>
       <c r="F5" t="inlineStr">
@@ -804,10 +805,10 @@
           <t>01:32:21</t>
         </is>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F6" t="inlineStr">
@@ -865,10 +866,10 @@
           <t>01:33:45</t>
         </is>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F7" t="inlineStr">
@@ -926,10 +927,10 @@
           <t>01:34:47</t>
         </is>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F8" t="inlineStr">
@@ -987,10 +988,10 @@
           <t>01:44:40</t>
         </is>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F9" t="inlineStr">
@@ -1048,10 +1049,10 @@
           <t>08:59:31</t>
         </is>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F10" t="inlineStr">
@@ -1109,10 +1110,10 @@
           <t>09:01:27</t>
         </is>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F11" t="inlineStr">
@@ -1170,10 +1171,10 @@
           <t>09:08:31</t>
         </is>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>45511</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="5" t="n">
         <v>45511</v>
       </c>
       <c r="F12" t="inlineStr">
@@ -1231,15 +1232,11 @@
           <t>15:10:44</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2024-08-22</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2024-08-22</t>
-        </is>
+      <c r="D13" s="5" t="n">
+        <v>45526</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>45526</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1281,6 +1278,71 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>20:20:04</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2024-08-26</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2024-08-26</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Cartographie</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ete</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>DroneA</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>